<commit_message>
StreamThread & StreamTask implementationé
</commit_message>
<xml_diff>
--- a/status_implementations.xlsx
+++ b/status_implementations.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\RepoPerso\kafka-stream-net\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{4DF837CA-976E-4772-BDD0-A2E1A6796213}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAAB3679-F5BA-4641-9AF1-A121C88E384A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{6BB3C3AC-BEBD-4971-9178-A48489FC2351}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="27">
   <si>
     <t>Stateless Operators</t>
   </si>
@@ -44,10 +44,6 @@
     <t>Filter</t>
   </si>
   <si>
-    <t>Kstream -&gt; Kstream
-Ktable -&gt; Ktable</t>
-  </si>
-  <si>
     <t>Inverse Filter</t>
   </si>
   <si>
@@ -66,10 +62,6 @@
     <t>KStream → void</t>
   </si>
   <si>
-    <t>KStream → void
-KTable → void</t>
-  </si>
-  <si>
     <t>GroupByKey</t>
   </si>
   <si>
@@ -79,20 +71,12 @@
     <t>GroupBy</t>
   </si>
   <si>
-    <t>KStream → KGroupedStream
-KTable → KGroupedTable</t>
-  </si>
-  <si>
     <t>Map</t>
   </si>
   <si>
     <t>MapValues</t>
   </si>
   <si>
-    <t>KStream → Kstream
-KTable → Ktable</t>
-  </si>
-  <si>
     <t>Peek</t>
   </si>
   <si>
@@ -112,6 +96,21 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Ktable -&gt; Ktable</t>
+  </si>
+  <si>
+    <t>Kstream -&gt; Kstream</t>
+  </si>
+  <si>
+    <t>KTable → void</t>
+  </si>
+  <si>
+    <t>KTable → KGroupedTable</t>
+  </si>
+  <si>
+    <t>KTable → Ktable</t>
   </si>
 </sst>
 </file>
@@ -143,7 +142,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -166,15 +165,38 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -184,6 +206,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -499,10 +530,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E398BEB-FCDF-4883-9C66-A7FB8D805E4F}">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -512,143 +543,183 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="5"/>
+      <c r="C1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="2"/>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="7"/>
+      <c r="B4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2"/>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="2"/>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="7"/>
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="2"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10" s="7"/>
+      <c r="B10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="2"/>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A13" s="7"/>
+      <c r="B13" s="3" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C3" s="3"/>
-    </row>
-    <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="3"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="3"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="3"/>
-    </row>
-    <row r="7" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="C14" s="2"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A15" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C15" s="2"/>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="7"/>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C17" s="2"/>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B18" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="3"/>
-    </row>
-    <row r="9" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="C9" s="3"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3"/>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="5" t="s">
+      <c r="C18" s="2"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C11" s="3"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="4" t="s">
+      <c r="B20" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="3"/>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C13" s="3"/>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C14" s="3"/>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C15" s="3"/>
+      <c r="C20" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="6">
+    <mergeCell ref="A15:A16"/>
     <mergeCell ref="A1:B1"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="A9:A10"/>
+    <mergeCell ref="A12:A13"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>